<commit_message>
updated with ertra vaccinated user fields
</commit_message>
<xml_diff>
--- a/src/asset/excel/vaccineexcel.xlsx
+++ b/src/asset/excel/vaccineexcel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -35,6 +35,18 @@
   </si>
   <si>
     <t xml:space="preserve">address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">department</t>
+  </si>
+  <si>
+    <t xml:space="preserve">company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joined date</t>
   </si>
   <si>
     <t xml:space="preserve">vaccineFirstDate</t>
@@ -55,9 +67,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="166" formatCode="0"/>
-    <numFmt numFmtId="167" formatCode="0.00"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -125,7 +137,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -138,7 +150,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -159,58 +175,72 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.26"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="2" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H2" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I7" s="3"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="3"/>
+      <c r="I2" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added product and change front view
</commit_message>
<xml_diff>
--- a/src/asset/excel/vaccineexcel.xlsx
+++ b/src/asset/excel/vaccineexcel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id number</t>
   </si>
   <si>
     <t xml:space="preserve">position</t>
@@ -175,7 +178,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
@@ -187,14 +190,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="11.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="12.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="15" style="2" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -219,10 +224,10 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -231,11 +236,14 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>